<commit_message>
Add Implement 4 service features
</commit_message>
<xml_diff>
--- a/data/templates/example_classification_input_user.xlsx
+++ b/data/templates/example_classification_input_user.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>n_sikap_A</t>
+          <t>n_sikap_a</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>mother_work_Lainnya</t>
+          <t>mother_work_lainnya</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -471,12 +471,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mother_salary_Sangat Rendah</t>
+          <t>mother_salary_sangat_rendah</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>father_salary_Tidak Berpenghasilan</t>
+          <t>father_salary_tidak_berpenghasilan</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -491,22 +491,22 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>father_edu_SMP sederajat</t>
+          <t>father_edu_smp_sederajat</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>father_work_Buruh</t>
+          <t>father_work_buruh</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>mother_salary_Cukup Rendah</t>
+          <t>mother_salary_cukup_rendah</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>mother_work_Buruh</t>
+          <t>mother_work_buruh</t>
         </is>
       </c>
     </row>

</xml_diff>